<commit_message>
:truck:[Move or Rename] SQL 디렉터리 정리
</commit_message>
<xml_diff>
--- a/1. PS/4. 복습 1회/코딩테스트 복습주기.xlsx
+++ b/1. PS/4. 복습 1회/코딩테스트 복습주기.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CloudStation\SourceCode\PS\1. PS\4. 복습 1회\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E0995D-ACBC-4AA5-BCE1-56292DBF6D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AF1684-65CF-4F99-8D7C-A4584A095481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{3D736860-356B-417E-8D4E-E79E65CE9C17}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
   <si>
     <t>0 / 1 / 4 / 7 / 14 / 30</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -601,6 +601,54 @@
     </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>정렬 - Q25. 실패율</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">정렬 - Q23. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>국영수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Q24. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>안테나</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>정렬 - Q27_정렬된 배열에서 특정 수의 개수 구하기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -609,7 +657,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -661,6 +709,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -1228,7 +1283,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1307,119 +1362,122 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1745,11 +1803,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC61086F-FA6B-47FC-85D4-709DD8996956}">
   <dimension ref="A1:AT84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z26" sqref="Z26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="4.58203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.58203125" style="2" bestFit="1" customWidth="1"/>
@@ -1771,85 +1829,85 @@
     <col min="47" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="83" t="s">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="17.5" thickBot="1">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="84"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85" t="s">
+      <c r="E1" s="61"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="85"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84" t="s">
+      <c r="H1" s="62"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84" t="s">
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84" t="s">
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72" t="s">
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="73"/>
-      <c r="AD1" s="73"/>
-      <c r="AE1" s="73"/>
-      <c r="AF1" s="73"/>
-      <c r="AG1" s="73"/>
-      <c r="AH1" s="73"/>
-      <c r="AI1" s="73"/>
-      <c r="AJ1" s="73"/>
-    </row>
-    <row r="2" spans="1:36" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="74" t="s">
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="50"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="50"/>
+    </row>
+    <row r="2" spans="1:36" ht="18" thickTop="1" thickBot="1">
+      <c r="A2" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="76" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="77"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="79" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="80"/>
-      <c r="H2" s="81"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="75"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="58"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="52"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:36" s="5" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="56" t="s">
+    <row r="3" spans="1:36" s="5" customFormat="1" ht="18" thickTop="1" thickBot="1">
+      <c r="A3" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="37"/>
       <c r="D3" s="37" t="s">
         <v>10</v>
@@ -1868,26 +1926,26 @@
       </c>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="58" t="s">
+      <c r="N3" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
-      <c r="R3" s="59"/>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="60"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="69"/>
       <c r="V3" s="27"/>
     </row>
-    <row r="4" spans="1:36" s="7" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="56" t="s">
+    <row r="4" spans="1:36" s="7" customFormat="1" ht="34.5" thickBot="1">
+      <c r="A4" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="56"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="5"/>
       <c r="D4" s="43" t="s">
         <v>13</v>
@@ -1906,20 +1964,20 @@
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="62"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="62"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="62"/>
-      <c r="T4" s="62"/>
-      <c r="U4" s="63"/>
+      <c r="N4" s="70"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="71"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="72"/>
       <c r="V4" s="28"/>
     </row>
-    <row r="5" spans="1:36" s="14" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.8">
+    <row r="5" spans="1:36" s="14" customFormat="1" ht="42" customHeight="1" thickBot="1">
       <c r="A5" s="16"/>
       <c r="B5" s="25" t="s">
         <v>39</v>
@@ -1939,15 +1997,15 @@
       <c r="G5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="70"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="64" t="s">
+      <c r="I5" s="82"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="65"/>
+      <c r="L5" s="74"/>
       <c r="M5" s="22" t="s">
         <v>31</v>
       </c>
@@ -1961,7 +2019,7 @@
       <c r="U5" s="15"/>
       <c r="V5" s="26"/>
     </row>
-    <row r="6" spans="1:36" s="8" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:36" s="8" customFormat="1" ht="18" thickTop="1" thickBot="1">
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
@@ -1983,14 +2041,14 @@
       <c r="G6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="66" t="s">
+      <c r="H6" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="68"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="77"/>
       <c r="N6" s="8" t="s">
         <v>14</v>
       </c>
@@ -2014,7 +2072,7 @@
       </c>
       <c r="V6" s="29"/>
     </row>
-    <row r="7" spans="1:36" ht="39.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:36" ht="39.5" customHeight="1" thickTop="1">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -2029,12 +2087,12 @@
       <c r="I7" s="11">
         <v>44417</v>
       </c>
-      <c r="J7" s="52" t="s">
+      <c r="J7" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="51"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="64"/>
       <c r="N7" s="2">
         <v>1</v>
       </c>
@@ -2065,7 +2123,7 @@
       <c r="AC7" s="32"/>
       <c r="AD7" s="32"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:36">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -2082,12 +2140,12 @@
       <c r="I8" s="11">
         <v>44418</v>
       </c>
-      <c r="J8" s="50" t="s">
+      <c r="J8" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="51"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="64"/>
       <c r="N8" s="2">
         <v>2</v>
       </c>
@@ -2103,7 +2161,7 @@
       <c r="Z8" s="9"/>
       <c r="AA8" s="9"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:36">
       <c r="A9" s="2">
         <v>3</v>
       </c>
@@ -2120,12 +2178,12 @@
       <c r="I9" s="11">
         <v>44419</v>
       </c>
-      <c r="J9" s="54" t="s">
+      <c r="J9" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
-      <c r="M9" s="55"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="80"/>
       <c r="N9" s="2">
         <v>3</v>
       </c>
@@ -2158,7 +2216,7 @@
       </c>
       <c r="AC9" s="33"/>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:36">
       <c r="A10" s="2">
         <v>4</v>
       </c>
@@ -2177,12 +2235,12 @@
       <c r="I10" s="11">
         <v>44423</v>
       </c>
-      <c r="J10" s="50" t="s">
+      <c r="J10" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="51"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="64"/>
       <c r="N10" s="2">
         <v>4</v>
       </c>
@@ -2202,7 +2260,7 @@
       <c r="AA10" s="9"/>
       <c r="AB10" s="9"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:36">
       <c r="A11" s="2">
         <v>5</v>
       </c>
@@ -2221,12 +2279,12 @@
       <c r="I11" s="11">
         <v>44424</v>
       </c>
-      <c r="J11" s="50" t="s">
+      <c r="J11" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="51"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="64"/>
       <c r="N11" s="2">
         <v>5</v>
       </c>
@@ -2261,7 +2319,7 @@
         <v>44436</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:36">
       <c r="A12" s="2">
         <v>6</v>
       </c>
@@ -2306,7 +2364,7 @@
       <c r="AA12" s="14"/>
       <c r="AB12" s="35"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:36">
       <c r="A13" s="2">
         <v>7</v>
       </c>
@@ -2325,12 +2383,12 @@
       <c r="I13" s="11">
         <v>44426</v>
       </c>
-      <c r="J13" s="50" t="s">
+      <c r="J13" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="51"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="63"/>
+      <c r="M13" s="64"/>
       <c r="N13" s="2">
         <v>7</v>
       </c>
@@ -2365,7 +2423,7 @@
         <v>44443</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:36">
       <c r="A14" s="2">
         <v>8</v>
       </c>
@@ -2416,7 +2474,7 @@
       <c r="AA14" s="35"/>
       <c r="AB14" s="35"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:36">
       <c r="A15" s="2">
         <v>9</v>
       </c>
@@ -2438,12 +2496,12 @@
       <c r="I15" s="11">
         <v>44429</v>
       </c>
-      <c r="J15" s="50" t="s">
+      <c r="J15" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="51"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="64"/>
       <c r="N15" s="2">
         <v>9</v>
       </c>
@@ -2481,7 +2539,7 @@
         <v>44450</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:36">
       <c r="A16" s="2">
         <v>10</v>
       </c>
@@ -2503,12 +2561,12 @@
       <c r="I16" s="11">
         <v>44431</v>
       </c>
-      <c r="J16" s="54" t="s">
+      <c r="J16" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="55"/>
+      <c r="K16" s="79"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="80"/>
       <c r="N16" s="2">
         <v>10</v>
       </c>
@@ -2531,7 +2589,7 @@
       <c r="AA16" s="14"/>
       <c r="AB16" s="14"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:32">
       <c r="A17" s="2">
         <v>11</v>
       </c>
@@ -2553,12 +2611,12 @@
       <c r="I17" s="11">
         <v>44433</v>
       </c>
-      <c r="J17" s="50" t="s">
+      <c r="J17" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="51"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="64"/>
       <c r="N17" s="2">
         <v>11</v>
       </c>
@@ -2596,7 +2654,7 @@
         <v>44457</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:32">
       <c r="A18" s="2">
         <v>12</v>
       </c>
@@ -2618,12 +2676,12 @@
       <c r="I18" s="11">
         <v>44434</v>
       </c>
-      <c r="J18" s="50" t="s">
+      <c r="J18" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="K18" s="50"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="51"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="64"/>
       <c r="N18" s="2">
         <v>12</v>
       </c>
@@ -2648,7 +2706,7 @@
       <c r="AA18" s="35"/>
       <c r="AB18" s="35"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:32">
       <c r="A19" s="2">
         <v>13</v>
       </c>
@@ -2670,12 +2728,12 @@
       <c r="I19" s="11">
         <v>44438</v>
       </c>
-      <c r="J19" s="54" t="s">
+      <c r="J19" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="55"/>
+      <c r="K19" s="79"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="80"/>
       <c r="N19" s="2">
         <v>13</v>
       </c>
@@ -2713,7 +2771,7 @@
         <v>44464</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:32">
       <c r="A20" s="2">
         <v>14</v>
       </c>
@@ -2735,12 +2793,12 @@
       <c r="I20" s="11">
         <v>44439</v>
       </c>
-      <c r="J20" s="50" t="s">
+      <c r="J20" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="51"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="64"/>
       <c r="N20" s="2">
         <v>14</v>
       </c>
@@ -2763,7 +2821,7 @@
       <c r="AA20" s="35"/>
       <c r="AB20" s="35"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:32">
       <c r="A21" s="2">
         <v>15</v>
       </c>
@@ -2788,12 +2846,12 @@
       <c r="I21" s="11">
         <v>44440</v>
       </c>
-      <c r="J21" s="54" t="s">
+      <c r="J21" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="55"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="79"/>
+      <c r="M21" s="80"/>
       <c r="N21" s="2">
         <v>15</v>
       </c>
@@ -2835,7 +2893,7 @@
         <v>44471</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:32">
       <c r="A22" s="2">
         <v>16</v>
       </c>
@@ -2860,12 +2918,12 @@
       <c r="I22" s="11">
         <v>44441</v>
       </c>
-      <c r="J22" s="54" t="s">
+      <c r="J22" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="55"/>
+      <c r="K22" s="79"/>
+      <c r="L22" s="79"/>
+      <c r="M22" s="80"/>
       <c r="N22" s="2">
         <v>16</v>
       </c>
@@ -2888,10 +2946,10 @@
       <c r="X22" s="35"/>
       <c r="Y22" s="47"/>
       <c r="Z22" s="47"/>
-      <c r="AA22" s="14"/>
+      <c r="AA22" s="47"/>
       <c r="AB22" s="14"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:32">
       <c r="A23" s="2">
         <v>17</v>
       </c>
@@ -2916,12 +2974,12 @@
       <c r="I23" s="11">
         <v>44442</v>
       </c>
-      <c r="J23" s="50" t="s">
+      <c r="J23" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="51"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="64"/>
       <c r="N23" s="2">
         <v>17</v>
       </c>
@@ -2943,14 +3001,26 @@
       <c r="V23" s="30">
         <v>44472</v>
       </c>
-      <c r="W23" s="14"/>
-      <c r="X23" s="14"/>
-      <c r="Y23" s="33"/>
-      <c r="Z23" s="33"/>
-      <c r="AA23" s="14"/>
-      <c r="AB23" s="14"/>
-    </row>
-    <row r="24" spans="1:32" s="38" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="W23" s="33">
+        <v>44473</v>
+      </c>
+      <c r="X23" s="33">
+        <v>44474</v>
+      </c>
+      <c r="Y23" s="33">
+        <v>44475</v>
+      </c>
+      <c r="Z23" s="33">
+        <v>44476</v>
+      </c>
+      <c r="AA23" s="33">
+        <v>44477</v>
+      </c>
+      <c r="AB23" s="33">
+        <v>44478</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" s="38" customFormat="1" ht="35" customHeight="1">
       <c r="A24" s="38">
         <v>18</v>
       </c>
@@ -2975,12 +3045,12 @@
       <c r="I24" s="41">
         <v>44443</v>
       </c>
-      <c r="J24" s="52" t="s">
+      <c r="J24" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="53"/>
+      <c r="K24" s="78"/>
+      <c r="L24" s="78"/>
+      <c r="M24" s="84"/>
       <c r="N24" s="38">
         <v>18</v>
       </c>
@@ -3001,9 +3071,10 @@
       </c>
       <c r="V24" s="42"/>
       <c r="Y24" s="41"/>
-      <c r="Z24" s="41"/>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="Z24" s="48"/>
+      <c r="AA24" s="48"/>
+    </row>
+    <row r="25" spans="1:32">
       <c r="A25" s="2">
         <v>19</v>
       </c>
@@ -3028,12 +3099,12 @@
       <c r="I25" s="11">
         <v>44445</v>
       </c>
-      <c r="J25" s="50" t="s">
+      <c r="J25" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="K25" s="50"/>
-      <c r="L25" s="50"/>
-      <c r="M25" s="51"/>
+      <c r="K25" s="63"/>
+      <c r="L25" s="63"/>
+      <c r="M25" s="64"/>
       <c r="N25" s="2">
         <v>19</v>
       </c>
@@ -3052,9 +3123,29 @@
       <c r="S25" s="11">
         <v>44445</v>
       </c>
-      <c r="Z25" s="11"/>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="V25" s="30">
+        <v>44479</v>
+      </c>
+      <c r="W25" s="33">
+        <v>44480</v>
+      </c>
+      <c r="X25" s="33">
+        <v>44481</v>
+      </c>
+      <c r="Y25" s="33">
+        <v>44482</v>
+      </c>
+      <c r="Z25" s="33">
+        <v>44483</v>
+      </c>
+      <c r="AA25" s="33">
+        <v>44484</v>
+      </c>
+      <c r="AB25" s="33">
+        <v>44485</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32">
       <c r="A26" s="2">
         <v>20</v>
       </c>
@@ -3079,12 +3170,12 @@
       <c r="I26" s="11">
         <v>44446</v>
       </c>
-      <c r="J26" s="50" t="s">
+      <c r="J26" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="K26" s="50"/>
-      <c r="L26" s="50"/>
-      <c r="M26" s="51"/>
+      <c r="K26" s="63"/>
+      <c r="L26" s="63"/>
+      <c r="M26" s="64"/>
       <c r="N26" s="2">
         <v>20</v>
       </c>
@@ -3106,7 +3197,7 @@
       <c r="AA26" s="11"/>
       <c r="AB26" s="11"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:32">
       <c r="A27" s="2">
         <v>21</v>
       </c>
@@ -3131,12 +3222,12 @@
       <c r="I27" s="11">
         <v>44447</v>
       </c>
-      <c r="J27" s="50" t="s">
+      <c r="J27" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="51"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="64"/>
       <c r="N27" s="2">
         <v>21</v>
       </c>
@@ -3155,10 +3246,29 @@
       <c r="S27" s="11">
         <v>44447</v>
       </c>
-      <c r="AB27" s="11"/>
-      <c r="AC27" s="11"/>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="V27" s="30">
+        <v>44486</v>
+      </c>
+      <c r="W27" s="33">
+        <v>44487</v>
+      </c>
+      <c r="X27" s="33">
+        <v>44488</v>
+      </c>
+      <c r="Y27" s="33">
+        <v>44489</v>
+      </c>
+      <c r="Z27" s="33">
+        <v>44490</v>
+      </c>
+      <c r="AA27" s="33">
+        <v>44491</v>
+      </c>
+      <c r="AB27" s="33">
+        <v>44492</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32">
       <c r="A28" s="2">
         <v>22</v>
       </c>
@@ -3183,12 +3293,12 @@
       <c r="I28" s="11">
         <v>44448</v>
       </c>
-      <c r="J28" s="50" t="s">
+      <c r="J28" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="K28" s="50"/>
-      <c r="L28" s="50"/>
-      <c r="M28" s="51"/>
+      <c r="K28" s="63"/>
+      <c r="L28" s="63"/>
+      <c r="M28" s="64"/>
       <c r="N28" s="2">
         <v>22</v>
       </c>
@@ -3209,7 +3319,7 @@
       </c>
       <c r="AC28" s="11"/>
     </row>
-    <row r="29" spans="1:32" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:32" ht="16.5" customHeight="1">
       <c r="A29" s="2">
         <v>23</v>
       </c>
@@ -3234,12 +3344,12 @@
       <c r="I29" s="11">
         <v>44452</v>
       </c>
-      <c r="J29" s="50" t="s">
+      <c r="J29" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="K29" s="50"/>
-      <c r="L29" s="50"/>
-      <c r="M29" s="51"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="63"/>
+      <c r="M29" s="64"/>
       <c r="N29" s="2">
         <v>23</v>
       </c>
@@ -3259,10 +3369,29 @@
         <v>44452</v>
       </c>
       <c r="U29" s="11"/>
-      <c r="V29" s="30"/>
-      <c r="W29" s="11"/>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="V29" s="30">
+        <v>44493</v>
+      </c>
+      <c r="W29" s="33">
+        <v>44494</v>
+      </c>
+      <c r="X29" s="33">
+        <v>44495</v>
+      </c>
+      <c r="Y29" s="33">
+        <v>44496</v>
+      </c>
+      <c r="Z29" s="33">
+        <v>44497</v>
+      </c>
+      <c r="AA29" s="33">
+        <v>44498</v>
+      </c>
+      <c r="AB29" s="33">
+        <v>44499</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32">
       <c r="A30" s="2">
         <v>24</v>
       </c>
@@ -3287,12 +3416,12 @@
       <c r="I30" s="11">
         <v>44453</v>
       </c>
-      <c r="J30" s="50" t="s">
+      <c r="J30" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="K30" s="50"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="51"/>
+      <c r="K30" s="63"/>
+      <c r="L30" s="63"/>
+      <c r="M30" s="64"/>
       <c r="N30" s="2">
         <v>24</v>
       </c>
@@ -3315,7 +3444,7 @@
       <c r="AD30" s="11"/>
       <c r="AE30" s="11"/>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:32">
       <c r="A31" s="2">
         <v>25</v>
       </c>
@@ -3340,12 +3469,12 @@
       <c r="I31" s="11">
         <v>44454</v>
       </c>
-      <c r="J31" s="50" t="s">
+      <c r="J31" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="51"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="63"/>
+      <c r="M31" s="64"/>
       <c r="N31" s="2">
         <v>25</v>
       </c>
@@ -3364,11 +3493,37 @@
       <c r="S31" s="11">
         <v>44454</v>
       </c>
-      <c r="AD31" s="11"/>
+      <c r="V31" s="30">
+        <v>44500</v>
+      </c>
+      <c r="W31" s="33">
+        <v>44501</v>
+      </c>
+      <c r="X31" s="33">
+        <v>44502</v>
+      </c>
+      <c r="Y31" s="33">
+        <v>44503</v>
+      </c>
+      <c r="Z31" s="33">
+        <v>44504</v>
+      </c>
+      <c r="AA31" s="33">
+        <v>44505</v>
+      </c>
+      <c r="AB31" s="33">
+        <v>44506</v>
+      </c>
+      <c r="AC31" s="33">
+        <v>44507</v>
+      </c>
+      <c r="AD31" s="33">
+        <v>44508</v>
+      </c>
       <c r="AE31" s="11"/>
       <c r="AF31" s="11"/>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:32">
       <c r="A32" s="2">
         <v>26</v>
       </c>
@@ -3393,12 +3548,12 @@
       <c r="I32" s="11">
         <v>44455</v>
       </c>
-      <c r="J32" s="50" t="s">
+      <c r="J32" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="K32" s="50"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="51"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="64"/>
       <c r="N32" s="2">
         <v>26</v>
       </c>
@@ -3421,7 +3576,7 @@
       <c r="AE32" s="11"/>
       <c r="AF32" s="11"/>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:43">
       <c r="A33" s="2">
         <v>27</v>
       </c>
@@ -3446,12 +3601,12 @@
       <c r="I33" s="11">
         <v>44456</v>
       </c>
-      <c r="J33" s="50" t="s">
+      <c r="J33" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="K33" s="50"/>
-      <c r="L33" s="50"/>
-      <c r="M33" s="51"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="64"/>
       <c r="N33" s="2">
         <v>27</v>
       </c>
@@ -3474,7 +3629,7 @@
       <c r="AE33" s="11"/>
       <c r="AF33" s="11"/>
     </row>
-    <row r="34" spans="1:43" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:43" ht="33.5" customHeight="1">
       <c r="A34" s="2">
         <v>28</v>
       </c>
@@ -3499,12 +3654,12 @@
       <c r="I34" s="11">
         <v>44460</v>
       </c>
-      <c r="J34" s="52" t="s">
+      <c r="J34" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="K34" s="50"/>
-      <c r="L34" s="50"/>
-      <c r="M34" s="51"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="64"/>
       <c r="N34" s="2">
         <v>28</v>
       </c>
@@ -3527,7 +3682,7 @@
       <c r="Z34" s="11"/>
       <c r="AF34" s="11"/>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:43">
       <c r="A35" s="2">
         <v>29</v>
       </c>
@@ -3552,12 +3707,12 @@
       <c r="I35" s="11">
         <v>44461</v>
       </c>
-      <c r="J35" s="50" t="s">
+      <c r="J35" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="K35" s="50"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="51"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="63"/>
+      <c r="M35" s="64"/>
       <c r="N35" s="2">
         <v>29</v>
       </c>
@@ -3580,7 +3735,7 @@
       <c r="AH35" s="11"/>
       <c r="AI35" s="11"/>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:43">
       <c r="A36" s="2">
         <v>30</v>
       </c>
@@ -3605,12 +3760,12 @@
       <c r="I36" s="11">
         <v>44462</v>
       </c>
-      <c r="J36" s="50" t="s">
+      <c r="J36" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="K36" s="50"/>
-      <c r="L36" s="50"/>
-      <c r="M36" s="51"/>
+      <c r="K36" s="63"/>
+      <c r="L36" s="63"/>
+      <c r="M36" s="64"/>
       <c r="N36" s="2">
         <v>30</v>
       </c>
@@ -3633,7 +3788,7 @@
       <c r="AI36" s="11"/>
       <c r="AJ36" s="11"/>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:43">
       <c r="A37" s="2">
         <v>31</v>
       </c>
@@ -3661,12 +3816,12 @@
       <c r="I37" s="11">
         <v>44463</v>
       </c>
-      <c r="J37" s="50" t="s">
+      <c r="J37" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="K37" s="50"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="51"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="63"/>
+      <c r="M37" s="64"/>
       <c r="N37" s="2">
         <v>31</v>
       </c>
@@ -3691,7 +3846,7 @@
       <c r="AI37" s="11"/>
       <c r="AJ37" s="11"/>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:43">
       <c r="A38" s="2">
         <v>32</v>
       </c>
@@ -3717,14 +3872,14 @@
         <v>32</v>
       </c>
       <c r="I38" s="11">
-        <v>44464</v>
-      </c>
-      <c r="J38" s="50" t="s">
+        <v>44466</v>
+      </c>
+      <c r="J38" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="K38" s="50"/>
-      <c r="L38" s="50"/>
-      <c r="M38" s="51"/>
+      <c r="K38" s="63"/>
+      <c r="L38" s="63"/>
+      <c r="M38" s="64"/>
       <c r="N38" s="2">
         <v>32</v>
       </c>
@@ -3748,7 +3903,7 @@
       </c>
       <c r="AJ38" s="11"/>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:43">
       <c r="A39" s="2">
         <v>33</v>
       </c>
@@ -3774,14 +3929,14 @@
         <v>33</v>
       </c>
       <c r="I39" s="11">
-        <v>44465</v>
-      </c>
-      <c r="J39" s="50" t="s">
+        <v>44468</v>
+      </c>
+      <c r="J39" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="K39" s="50"/>
-      <c r="L39" s="50"/>
-      <c r="M39" s="51"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="63"/>
+      <c r="M39" s="64"/>
       <c r="N39" s="2">
         <v>33</v>
       </c>
@@ -3805,14 +3960,14 @@
       </c>
       <c r="AK39" s="11"/>
     </row>
-    <row r="40" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:43">
       <c r="A40" s="2">
         <v>34</v>
       </c>
       <c r="B40" s="9">
         <v>33</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="9">
         <v>34</v>
       </c>
       <c r="D40" s="9">
@@ -3831,19 +3986,23 @@
         <v>34</v>
       </c>
       <c r="I40" s="11">
-        <v>44466</v>
-      </c>
-      <c r="J40" s="48"/>
-      <c r="K40" s="48"/>
-      <c r="L40" s="48"/>
-      <c r="M40" s="49"/>
+        <v>44469</v>
+      </c>
+      <c r="J40" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="K40" s="63"/>
+      <c r="L40" s="63"/>
+      <c r="M40" s="64"/>
       <c r="N40" s="2">
         <v>34</v>
       </c>
       <c r="O40" s="11">
         <v>44469</v>
       </c>
-      <c r="P40" s="11"/>
+      <c r="P40" s="11">
+        <v>44469</v>
+      </c>
       <c r="Q40" s="11">
         <v>44469</v>
       </c>
@@ -3859,85 +4018,125 @@
       <c r="AK40" s="11"/>
       <c r="AL40" s="11"/>
     </row>
-    <row r="41" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:43">
       <c r="A41" s="2">
         <v>35</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="9">
         <v>34</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="9">
         <v>35</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="9">
         <v>32</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="9">
         <v>28</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="9">
         <v>21</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="9">
         <v>5</v>
       </c>
       <c r="H41" s="10">
         <v>35</v>
       </c>
       <c r="I41" s="11">
-        <v>44467</v>
-      </c>
-      <c r="J41" s="48"/>
-      <c r="K41" s="48"/>
-      <c r="L41" s="48"/>
-      <c r="M41" s="49"/>
+        <v>44476</v>
+      </c>
+      <c r="J41" s="63" t="s">
+        <v>72</v>
+      </c>
+      <c r="K41" s="63"/>
+      <c r="L41" s="63"/>
+      <c r="M41" s="64"/>
       <c r="N41" s="2">
         <v>35</v>
+      </c>
+      <c r="O41" s="11">
+        <v>44476</v>
+      </c>
+      <c r="P41" s="11">
+        <v>44476</v>
+      </c>
+      <c r="Q41" s="11">
+        <v>44476</v>
+      </c>
+      <c r="R41" s="11">
+        <v>44476</v>
+      </c>
+      <c r="S41" s="11">
+        <v>44476</v>
+      </c>
+      <c r="T41" s="11">
+        <v>44476</v>
       </c>
       <c r="AL41" s="11"/>
       <c r="AM41" s="11"/>
       <c r="AN41" s="11"/>
     </row>
-    <row r="42" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:43">
       <c r="A42" s="2">
         <v>36</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="9">
         <v>35</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="9">
         <v>36</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="9">
         <v>33</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="9">
         <v>29</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="9">
         <v>22</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="9">
         <v>6</v>
       </c>
       <c r="H42" s="10">
         <v>36</v>
       </c>
       <c r="I42" s="11">
-        <v>44468</v>
-      </c>
-      <c r="J42" s="48"/>
-      <c r="K42" s="48"/>
-      <c r="L42" s="48"/>
-      <c r="M42" s="49"/>
+        <v>44477</v>
+      </c>
+      <c r="J42" s="63" t="s">
+        <v>74</v>
+      </c>
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="64"/>
       <c r="N42" s="2">
         <v>36</v>
+      </c>
+      <c r="O42" s="11">
+        <v>44477</v>
+      </c>
+      <c r="P42" s="11">
+        <v>44477</v>
+      </c>
+      <c r="Q42" s="11">
+        <v>44477</v>
+      </c>
+      <c r="R42" s="11">
+        <v>44477</v>
+      </c>
+      <c r="S42" s="11">
+        <v>44477</v>
+      </c>
+      <c r="T42" s="11">
+        <v>44477</v>
       </c>
       <c r="AL42" s="11"/>
       <c r="AM42" s="11"/>
       <c r="AN42" s="11"/>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:43">
       <c r="A43" s="2">
         <v>37</v>
       </c>
@@ -3963,19 +4162,19 @@
         <v>37</v>
       </c>
       <c r="I43" s="11">
-        <v>44469</v>
-      </c>
-      <c r="J43" s="48"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="48"/>
-      <c r="M43" s="49"/>
+        <v>44478</v>
+      </c>
+      <c r="J43" s="85"/>
+      <c r="K43" s="85"/>
+      <c r="L43" s="85"/>
+      <c r="M43" s="86"/>
       <c r="N43" s="2">
         <v>37</v>
       </c>
       <c r="AM43" s="11"/>
       <c r="AN43" s="11"/>
     </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:43">
       <c r="A44" s="2">
         <v>38</v>
       </c>
@@ -4001,12 +4200,12 @@
         <v>38</v>
       </c>
       <c r="I44" s="11">
-        <v>44470</v>
-      </c>
-      <c r="J44" s="48"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="48"/>
-      <c r="M44" s="49"/>
+        <v>44479</v>
+      </c>
+      <c r="J44" s="85"/>
+      <c r="K44" s="85"/>
+      <c r="L44" s="85"/>
+      <c r="M44" s="86"/>
       <c r="N44" s="2">
         <v>38</v>
       </c>
@@ -4014,7 +4213,7 @@
       <c r="AN44" s="11"/>
       <c r="AO44" s="11"/>
     </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:43">
       <c r="A45" s="2">
         <v>39</v>
       </c>
@@ -4040,12 +4239,12 @@
         <v>39</v>
       </c>
       <c r="I45" s="11">
-        <v>44471</v>
-      </c>
-      <c r="J45" s="48"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="48"/>
-      <c r="M45" s="49"/>
+        <v>44480</v>
+      </c>
+      <c r="J45" s="85"/>
+      <c r="K45" s="85"/>
+      <c r="L45" s="85"/>
+      <c r="M45" s="86"/>
       <c r="N45" s="2">
         <v>39</v>
       </c>
@@ -4053,7 +4252,7 @@
       <c r="AO45" s="11"/>
       <c r="AP45" s="11"/>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:43">
       <c r="A46" s="2">
         <v>40</v>
       </c>
@@ -4079,19 +4278,19 @@
         <v>40</v>
       </c>
       <c r="I46" s="11">
-        <v>44472</v>
-      </c>
-      <c r="J46" s="48"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="48"/>
-      <c r="M46" s="49"/>
+        <v>44481</v>
+      </c>
+      <c r="J46" s="85"/>
+      <c r="K46" s="85"/>
+      <c r="L46" s="85"/>
+      <c r="M46" s="86"/>
       <c r="N46" s="2">
         <v>40</v>
       </c>
       <c r="AO46" s="11"/>
       <c r="AP46" s="11"/>
     </row>
-    <row r="47" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:43">
       <c r="A47" s="2">
         <v>41</v>
       </c>
@@ -4117,19 +4316,19 @@
         <v>41</v>
       </c>
       <c r="I47" s="11">
-        <v>44473</v>
-      </c>
-      <c r="J47" s="48"/>
-      <c r="K47" s="48"/>
-      <c r="L47" s="48"/>
-      <c r="M47" s="49"/>
+        <v>44482</v>
+      </c>
+      <c r="J47" s="85"/>
+      <c r="K47" s="85"/>
+      <c r="L47" s="85"/>
+      <c r="M47" s="86"/>
       <c r="N47" s="2">
         <v>41</v>
       </c>
       <c r="AP47" s="11"/>
       <c r="AQ47" s="11"/>
     </row>
-    <row r="48" spans="1:43" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:43">
       <c r="A48" s="2">
         <v>42</v>
       </c>
@@ -4155,19 +4354,19 @@
         <v>42</v>
       </c>
       <c r="I48" s="11">
-        <v>44474</v>
-      </c>
-      <c r="J48" s="48"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="48"/>
-      <c r="M48" s="49"/>
+        <v>44483</v>
+      </c>
+      <c r="J48" s="85"/>
+      <c r="K48" s="85"/>
+      <c r="L48" s="85"/>
+      <c r="M48" s="86"/>
       <c r="N48" s="2">
         <v>42</v>
       </c>
       <c r="AP48" s="11"/>
       <c r="AQ48" s="11"/>
     </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:46">
       <c r="A49" s="2">
         <v>43</v>
       </c>
@@ -4193,12 +4392,12 @@
         <v>43</v>
       </c>
       <c r="I49" s="11">
-        <v>44475</v>
-      </c>
-      <c r="J49" s="48"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48"/>
-      <c r="M49" s="49"/>
+        <v>44484</v>
+      </c>
+      <c r="J49" s="85"/>
+      <c r="K49" s="85"/>
+      <c r="L49" s="85"/>
+      <c r="M49" s="86"/>
       <c r="N49" s="2">
         <v>43</v>
       </c>
@@ -4206,7 +4405,7 @@
       <c r="AQ49" s="11"/>
       <c r="AR49" s="11"/>
     </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:46">
       <c r="A50" s="2">
         <v>44</v>
       </c>
@@ -4232,12 +4431,12 @@
         <v>44</v>
       </c>
       <c r="I50" s="11">
-        <v>44476</v>
-      </c>
-      <c r="J50" s="48"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="48"/>
-      <c r="M50" s="49"/>
+        <v>44485</v>
+      </c>
+      <c r="J50" s="85"/>
+      <c r="K50" s="85"/>
+      <c r="L50" s="85"/>
+      <c r="M50" s="86"/>
       <c r="N50" s="2">
         <v>44</v>
       </c>
@@ -4245,7 +4444,7 @@
       <c r="AR50" s="11"/>
       <c r="AS50" s="11"/>
     </row>
-    <row r="51" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:46">
       <c r="A51" s="2">
         <v>45</v>
       </c>
@@ -4271,12 +4470,12 @@
         <v>45</v>
       </c>
       <c r="I51" s="11">
-        <v>44477</v>
-      </c>
-      <c r="J51" s="48"/>
-      <c r="K51" s="48"/>
-      <c r="L51" s="48"/>
-      <c r="M51" s="49"/>
+        <v>44486</v>
+      </c>
+      <c r="J51" s="85"/>
+      <c r="K51" s="85"/>
+      <c r="L51" s="85"/>
+      <c r="M51" s="86"/>
       <c r="N51" s="2">
         <v>45</v>
       </c>
@@ -4284,7 +4483,7 @@
       <c r="AS51" s="11"/>
       <c r="AT51" s="11"/>
     </row>
-    <row r="52" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:46">
       <c r="A52" s="2">
         <v>46</v>
       </c>
@@ -4310,12 +4509,12 @@
         <v>46</v>
       </c>
       <c r="I52" s="11">
-        <v>44478</v>
-      </c>
-      <c r="J52" s="48"/>
-      <c r="K52" s="48"/>
-      <c r="L52" s="48"/>
-      <c r="M52" s="49"/>
+        <v>44487</v>
+      </c>
+      <c r="J52" s="85"/>
+      <c r="K52" s="85"/>
+      <c r="L52" s="85"/>
+      <c r="M52" s="86"/>
       <c r="N52" s="2">
         <v>46</v>
       </c>
@@ -4323,7 +4522,7 @@
       <c r="AS52" s="11"/>
       <c r="AT52" s="11"/>
     </row>
-    <row r="53" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:46">
       <c r="A53" s="2">
         <v>47</v>
       </c>
@@ -4346,12 +4545,12 @@
         <v>47</v>
       </c>
       <c r="I53" s="11">
-        <v>44479</v>
-      </c>
-      <c r="J53" s="48"/>
-      <c r="K53" s="48"/>
-      <c r="L53" s="48"/>
-      <c r="M53" s="49"/>
+        <v>44488</v>
+      </c>
+      <c r="J53" s="85"/>
+      <c r="K53" s="85"/>
+      <c r="L53" s="85"/>
+      <c r="M53" s="86"/>
       <c r="N53" s="2">
         <v>47</v>
       </c>
@@ -4359,7 +4558,7 @@
       <c r="AS53" s="11"/>
       <c r="AT53" s="11"/>
     </row>
-    <row r="54" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:46">
       <c r="A54" s="2">
         <v>48</v>
       </c>
@@ -4379,12 +4578,12 @@
         <v>48</v>
       </c>
       <c r="I54" s="11">
-        <v>44480</v>
-      </c>
-      <c r="J54" s="48"/>
-      <c r="K54" s="48"/>
-      <c r="L54" s="48"/>
-      <c r="M54" s="49"/>
+        <v>44489</v>
+      </c>
+      <c r="J54" s="85"/>
+      <c r="K54" s="85"/>
+      <c r="L54" s="85"/>
+      <c r="M54" s="86"/>
       <c r="N54" s="2">
         <v>48</v>
       </c>
@@ -4392,7 +4591,7 @@
       <c r="W54" s="11"/>
       <c r="AT54" s="11"/>
     </row>
-    <row r="55" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:46">
       <c r="A55" s="2">
         <v>49</v>
       </c>
@@ -4412,12 +4611,12 @@
         <v>49</v>
       </c>
       <c r="I55" s="11">
-        <v>44481</v>
-      </c>
-      <c r="J55" s="48"/>
-      <c r="K55" s="48"/>
-      <c r="L55" s="48"/>
-      <c r="M55" s="49"/>
+        <v>44490</v>
+      </c>
+      <c r="J55" s="85"/>
+      <c r="K55" s="85"/>
+      <c r="L55" s="85"/>
+      <c r="M55" s="86"/>
       <c r="N55" s="2">
         <v>49</v>
       </c>
@@ -4425,7 +4624,7 @@
       <c r="Y55" s="11"/>
       <c r="Z55" s="11"/>
     </row>
-    <row r="56" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:46">
       <c r="A56" s="2">
         <v>50</v>
       </c>
@@ -4442,12 +4641,12 @@
         <v>50</v>
       </c>
       <c r="I56" s="11">
-        <v>44482</v>
-      </c>
-      <c r="J56" s="48"/>
-      <c r="K56" s="48"/>
-      <c r="L56" s="48"/>
-      <c r="M56" s="49"/>
+        <v>44491</v>
+      </c>
+      <c r="J56" s="85"/>
+      <c r="K56" s="85"/>
+      <c r="L56" s="85"/>
+      <c r="M56" s="86"/>
       <c r="N56" s="2">
         <v>50</v>
       </c>
@@ -4455,7 +4654,7 @@
       <c r="AB56" s="11"/>
       <c r="AC56" s="11"/>
     </row>
-    <row r="57" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:46">
       <c r="A57" s="2">
         <v>51</v>
       </c>
@@ -4472,12 +4671,12 @@
         <v>51</v>
       </c>
       <c r="I57" s="11">
-        <v>44483</v>
-      </c>
-      <c r="J57" s="48"/>
-      <c r="K57" s="48"/>
-      <c r="L57" s="48"/>
-      <c r="M57" s="49"/>
+        <v>44492</v>
+      </c>
+      <c r="J57" s="85"/>
+      <c r="K57" s="85"/>
+      <c r="L57" s="85"/>
+      <c r="M57" s="86"/>
       <c r="N57" s="2">
         <v>51</v>
       </c>
@@ -4485,7 +4684,7 @@
       <c r="AB57" s="11"/>
       <c r="AC57" s="11"/>
     </row>
-    <row r="58" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:46">
       <c r="A58" s="2">
         <v>52</v>
       </c>
@@ -4502,12 +4701,12 @@
         <v>52</v>
       </c>
       <c r="I58" s="11">
-        <v>44484</v>
-      </c>
-      <c r="J58" s="48"/>
-      <c r="K58" s="48"/>
-      <c r="L58" s="48"/>
-      <c r="M58" s="49"/>
+        <v>44493</v>
+      </c>
+      <c r="J58" s="85"/>
+      <c r="K58" s="85"/>
+      <c r="L58" s="85"/>
+      <c r="M58" s="86"/>
       <c r="N58" s="2">
         <v>52</v>
       </c>
@@ -4515,7 +4714,7 @@
       <c r="AE58" s="11"/>
       <c r="AF58" s="11"/>
     </row>
-    <row r="59" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:46">
       <c r="A59" s="2">
         <v>53</v>
       </c>
@@ -4532,12 +4731,12 @@
         <v>53</v>
       </c>
       <c r="I59" s="11">
-        <v>44485</v>
-      </c>
-      <c r="J59" s="48"/>
-      <c r="K59" s="48"/>
-      <c r="L59" s="48"/>
-      <c r="M59" s="49"/>
+        <v>44494</v>
+      </c>
+      <c r="J59" s="85"/>
+      <c r="K59" s="85"/>
+      <c r="L59" s="85"/>
+      <c r="M59" s="86"/>
       <c r="N59" s="2">
         <v>53</v>
       </c>
@@ -4545,7 +4744,7 @@
       <c r="AH59" s="11"/>
       <c r="AI59" s="11"/>
     </row>
-    <row r="60" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:46">
       <c r="A60" s="2">
         <v>54</v>
       </c>
@@ -4559,18 +4758,18 @@
         <v>54</v>
       </c>
       <c r="I60" s="11">
-        <v>44486</v>
-      </c>
-      <c r="J60" s="48"/>
-      <c r="K60" s="48"/>
-      <c r="L60" s="48"/>
-      <c r="M60" s="49"/>
+        <v>44495</v>
+      </c>
+      <c r="J60" s="85"/>
+      <c r="K60" s="85"/>
+      <c r="L60" s="85"/>
+      <c r="M60" s="86"/>
       <c r="N60" s="2">
         <v>54</v>
       </c>
       <c r="AJ60" s="11"/>
     </row>
-    <row r="61" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:46">
       <c r="A61" s="2">
         <v>55</v>
       </c>
@@ -4584,12 +4783,12 @@
         <v>55</v>
       </c>
       <c r="I61" s="11">
-        <v>44487</v>
-      </c>
-      <c r="J61" s="48"/>
-      <c r="K61" s="48"/>
-      <c r="L61" s="48"/>
-      <c r="M61" s="49"/>
+        <v>44496</v>
+      </c>
+      <c r="J61" s="85"/>
+      <c r="K61" s="85"/>
+      <c r="L61" s="85"/>
+      <c r="M61" s="86"/>
       <c r="N61" s="2">
         <v>55</v>
       </c>
@@ -4598,7 +4797,7 @@
       <c r="AM61" s="11"/>
       <c r="AN61" s="11"/>
     </row>
-    <row r="62" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:46">
       <c r="A62" s="2">
         <v>56</v>
       </c>
@@ -4612,12 +4811,12 @@
         <v>56</v>
       </c>
       <c r="I62" s="11">
-        <v>44488</v>
-      </c>
-      <c r="J62" s="48"/>
-      <c r="K62" s="48"/>
-      <c r="L62" s="48"/>
-      <c r="M62" s="49"/>
+        <v>44497</v>
+      </c>
+      <c r="J62" s="85"/>
+      <c r="K62" s="85"/>
+      <c r="L62" s="85"/>
+      <c r="M62" s="86"/>
       <c r="N62" s="2">
         <v>56</v>
       </c>
@@ -4625,7 +4824,7 @@
       <c r="AN62" s="11"/>
       <c r="AO62" s="11"/>
     </row>
-    <row r="63" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:46">
       <c r="A63" s="2">
         <v>57</v>
       </c>
@@ -4639,12 +4838,12 @@
         <v>57</v>
       </c>
       <c r="I63" s="11">
-        <v>44489</v>
-      </c>
-      <c r="J63" s="48"/>
-      <c r="K63" s="48"/>
-      <c r="L63" s="48"/>
-      <c r="M63" s="49"/>
+        <v>44498</v>
+      </c>
+      <c r="J63" s="85"/>
+      <c r="K63" s="85"/>
+      <c r="L63" s="85"/>
+      <c r="M63" s="86"/>
       <c r="N63" s="2">
         <v>57</v>
       </c>
@@ -4652,7 +4851,7 @@
       <c r="AQ63" s="11"/>
       <c r="AR63" s="11"/>
     </row>
-    <row r="64" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:46">
       <c r="A64" s="2">
         <v>58</v>
       </c>
@@ -4666,19 +4865,19 @@
         <v>58</v>
       </c>
       <c r="I64" s="11">
-        <v>44490</v>
-      </c>
-      <c r="J64" s="48"/>
-      <c r="K64" s="48"/>
-      <c r="L64" s="48"/>
-      <c r="M64" s="49"/>
+        <v>44499</v>
+      </c>
+      <c r="J64" s="85"/>
+      <c r="K64" s="85"/>
+      <c r="L64" s="85"/>
+      <c r="M64" s="86"/>
       <c r="N64" s="2">
         <v>58</v>
       </c>
       <c r="AS64" s="11"/>
       <c r="AT64" s="11"/>
     </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:44">
       <c r="A65" s="2">
         <v>59</v>
       </c>
@@ -4692,17 +4891,17 @@
         <v>59</v>
       </c>
       <c r="I65" s="11">
-        <v>44491</v>
-      </c>
-      <c r="J65" s="48"/>
-      <c r="K65" s="48"/>
-      <c r="L65" s="48"/>
-      <c r="M65" s="49"/>
+        <v>44500</v>
+      </c>
+      <c r="J65" s="85"/>
+      <c r="K65" s="85"/>
+      <c r="L65" s="85"/>
+      <c r="M65" s="86"/>
       <c r="N65" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:44">
       <c r="A66" s="2">
         <v>60</v>
       </c>
@@ -4716,17 +4915,17 @@
         <v>60</v>
       </c>
       <c r="I66" s="11">
-        <v>44492</v>
-      </c>
-      <c r="J66" s="48"/>
-      <c r="K66" s="48"/>
-      <c r="L66" s="48"/>
-      <c r="M66" s="49"/>
+        <v>44501</v>
+      </c>
+      <c r="J66" s="85"/>
+      <c r="K66" s="85"/>
+      <c r="L66" s="85"/>
+      <c r="M66" s="86"/>
       <c r="N66" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:44">
       <c r="A67" s="2">
         <v>61</v>
       </c>
@@ -4737,13 +4936,13 @@
         <v>61</v>
       </c>
       <c r="I67" s="11">
-        <v>44493</v>
+        <v>44502</v>
       </c>
       <c r="S67" s="11"/>
       <c r="T67" s="11"/>
       <c r="U67" s="11"/>
     </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:44">
       <c r="A68" s="2">
         <v>62</v>
       </c>
@@ -4754,13 +4953,13 @@
         <v>62</v>
       </c>
       <c r="I68" s="11">
-        <v>44494</v>
+        <v>44503</v>
       </c>
       <c r="U68" s="11"/>
       <c r="V68" s="30"/>
       <c r="W68" s="11"/>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:44">
       <c r="A69" s="2">
         <v>63</v>
       </c>
@@ -4771,12 +4970,12 @@
         <v>63</v>
       </c>
       <c r="I69" s="11">
-        <v>44495</v>
+        <v>44504</v>
       </c>
       <c r="W69" s="11"/>
       <c r="X69" s="11"/>
     </row>
-    <row r="70" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:44">
       <c r="A70" s="2">
         <v>64</v>
       </c>
@@ -4787,12 +4986,12 @@
         <v>64</v>
       </c>
       <c r="I70" s="11">
-        <v>44496</v>
+        <v>44505</v>
       </c>
       <c r="Y70" s="11"/>
       <c r="Z70" s="11"/>
     </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:44">
       <c r="A71" s="2">
         <v>65</v>
       </c>
@@ -4803,11 +5002,11 @@
         <v>65</v>
       </c>
       <c r="I71" s="11">
-        <v>44497</v>
+        <v>44506</v>
       </c>
       <c r="AA71" s="11"/>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:44">
       <c r="A72" s="2">
         <v>66</v>
       </c>
@@ -4818,12 +5017,12 @@
         <v>66</v>
       </c>
       <c r="I72" s="11">
-        <v>44498</v>
+        <v>44507</v>
       </c>
       <c r="AB72" s="11"/>
       <c r="AC72" s="11"/>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:44">
       <c r="A73" s="2">
         <v>67</v>
       </c>
@@ -4834,12 +5033,12 @@
         <v>67</v>
       </c>
       <c r="I73" s="11">
-        <v>44499</v>
+        <v>44508</v>
       </c>
       <c r="AD73" s="11"/>
       <c r="AE73" s="11"/>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:44">
       <c r="A74" s="2">
         <v>68</v>
       </c>
@@ -4850,12 +5049,12 @@
         <v>68</v>
       </c>
       <c r="I74" s="11">
-        <v>44500</v>
+        <v>44509</v>
       </c>
       <c r="AF74" s="11"/>
       <c r="AG74" s="11"/>
     </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:44">
       <c r="A75" s="2">
         <v>69</v>
       </c>
@@ -4866,11 +5065,11 @@
         <v>69</v>
       </c>
       <c r="I75" s="11">
-        <v>44501</v>
+        <v>44510</v>
       </c>
       <c r="AH75" s="11"/>
     </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:44">
       <c r="A76" s="2">
         <v>70</v>
       </c>
@@ -4881,12 +5080,12 @@
         <v>70</v>
       </c>
       <c r="I76" s="11">
-        <v>44502</v>
+        <v>44511</v>
       </c>
       <c r="AI76" s="11"/>
       <c r="AJ76" s="11"/>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:44">
       <c r="A77" s="2">
         <v>71</v>
       </c>
@@ -4897,12 +5096,12 @@
         <v>71</v>
       </c>
       <c r="I77" s="11">
-        <v>44503</v>
+        <v>44512</v>
       </c>
       <c r="AK77" s="11"/>
       <c r="AL77" s="11"/>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:44">
       <c r="A78" s="2">
         <v>72</v>
       </c>
@@ -4913,13 +5112,13 @@
         <v>72</v>
       </c>
       <c r="I78" s="11">
-        <v>44504</v>
+        <v>44513</v>
       </c>
       <c r="AM78" s="11"/>
       <c r="AN78" s="11"/>
       <c r="AO78" s="11"/>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:44">
       <c r="A79" s="2">
         <v>73</v>
       </c>
@@ -4930,12 +5129,12 @@
         <v>73</v>
       </c>
       <c r="I79" s="11">
-        <v>44505</v>
+        <v>44514</v>
       </c>
       <c r="AP79" s="11"/>
       <c r="AQ79" s="11"/>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:44">
       <c r="A80" s="2">
         <v>74</v>
       </c>
@@ -4946,11 +5145,11 @@
         <v>74</v>
       </c>
       <c r="I80" s="11">
-        <v>44506</v>
+        <v>44515</v>
       </c>
       <c r="AR80" s="11"/>
     </row>
-    <row r="81" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:46">
       <c r="A81" s="2">
         <v>75</v>
       </c>
@@ -4961,12 +5160,12 @@
         <v>75</v>
       </c>
       <c r="I81" s="11">
-        <v>44507</v>
+        <v>44516</v>
       </c>
       <c r="AS81" s="11"/>
       <c r="AT81" s="11"/>
     </row>
-    <row r="82" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:46">
       <c r="A82" s="2">
         <v>76</v>
       </c>
@@ -4977,32 +5176,73 @@
         <v>76</v>
       </c>
       <c r="I82" s="11">
-        <v>44508</v>
+        <v>44517</v>
       </c>
       <c r="M82" s="12"/>
       <c r="N82" s="11"/>
     </row>
-    <row r="83" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:46">
       <c r="O83" s="11"/>
     </row>
-    <row r="84" spans="1:46" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:46">
       <c r="P84" s="11"/>
       <c r="Q84" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="AB1:AJ1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="J66:M66"/>
+    <mergeCell ref="J60:M60"/>
+    <mergeCell ref="J61:M61"/>
+    <mergeCell ref="J62:M62"/>
+    <mergeCell ref="J63:M63"/>
+    <mergeCell ref="J64:M64"/>
+    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="J59:M59"/>
+    <mergeCell ref="J48:M48"/>
+    <mergeCell ref="J49:M49"/>
+    <mergeCell ref="J50:M50"/>
+    <mergeCell ref="J51:M51"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="J56:M56"/>
+    <mergeCell ref="J57:M57"/>
+    <mergeCell ref="J58:M58"/>
+    <mergeCell ref="J47:M47"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="J45:M45"/>
+    <mergeCell ref="J46:M46"/>
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="J22:M22"/>
     <mergeCell ref="J11:M11"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="K3:L3"/>
@@ -5016,59 +5256,18 @@
     <mergeCell ref="J9:M9"/>
     <mergeCell ref="J10:M10"/>
     <mergeCell ref="H5:J5"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="J29:M29"/>
-    <mergeCell ref="J30:M30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J47:M47"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="J45:M45"/>
-    <mergeCell ref="J46:M46"/>
-    <mergeCell ref="J59:M59"/>
-    <mergeCell ref="J48:M48"/>
-    <mergeCell ref="J49:M49"/>
-    <mergeCell ref="J50:M50"/>
-    <mergeCell ref="J51:M51"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="J55:M55"/>
-    <mergeCell ref="J56:M56"/>
-    <mergeCell ref="J57:M57"/>
-    <mergeCell ref="J58:M58"/>
-    <mergeCell ref="J66:M66"/>
-    <mergeCell ref="J60:M60"/>
-    <mergeCell ref="J61:M61"/>
-    <mergeCell ref="J62:M62"/>
-    <mergeCell ref="J63:M63"/>
-    <mergeCell ref="J64:M64"/>
-    <mergeCell ref="J65:M65"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="V1:AA1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>